<commit_message>
tencent finished and update excel operation
</commit_message>
<xml_diff>
--- a/预警通报爬取统计.xlsx
+++ b/预警通报爬取统计.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,1099 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2021-03-04</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>VMware View Planner 远程代码执行漏洞通告</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://cert.360.cn/warning/detail?id=a5ef2a08fd53b2c7519dd06c23f11242</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2021年03月04日，360CERT监测发现VMware发布了View Planner的风险通告，该漏洞编号为CVE-2021-21978，事件等级：高危，事件评分：8.6。View Planner 在处理上传文件时存在一处漏洞。该漏洞允许攻击者上传文件至任意目录，并在特定情况下导致远程代码执行。该漏洞poc已经公开对此，360CERT建议广大用户及时将view_planner升级到最新版本。与此同时，请做好资产自查以及预防工作，以免遭受黑客攻击。</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CVE-2021-21978: 文件上传漏洞VMware View Planner 的 web 上传接口中itrLogPath参数未进行严格的校验，允许攻击者实施目录穿越，将文件上传至任意目录。在攻击者上传恶意脚本文件覆盖特定的 web 程序执行脚本时，可造成远程代码执行。</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>通用修补建议下载并安装最新更新VMWare VMSA-2021-0003 安全通告</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-03-03</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>微软Exchange多个高危漏洞通告</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://cert.360.cn/warning/detail?id=f1439e4afc8b22a2c9b21a4ecc592f2f</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2021年03月03日，360CERT监测发现微软发布了Exchange 多个高危漏洞的风险通告，该漏洞编号为CVE-2021-26855,CVE-2021-26857,CVE-2021-26858,CVE-2021-27065，事件等级：严重，事件评分：9.8。对此，360CERT建议广大用户及时将exchange升级到最新版本。与此同时，请做好资产自查以及预防工作，以免遭受黑客攻击。</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CVE-2021-26855: 服务端请求伪造漏洞Exchange服务器端请求伪造（SSRF）漏洞，利用此漏洞的攻击者能够发送任意HTTP请求并通过Exchange Server进行身份验证。CVE-2021-26857: 序列化漏洞Exchange反序列化漏洞，该漏洞需要管理员权限，利用此漏洞的攻击者可以在Exchange服务器上以SYSTEM身份运行代码。CVE-2021-26858/CVE-2021-27065: 任意文件写入漏洞Exchange中身份验证后的任意文件写入漏洞。攻击者通过Exchange服务器进行身份验证后，可以利用此漏洞将文件写入服务器上的任何路径。该漏洞可以配合CVE-2021-26855 SSRF漏洞进行组合攻击。</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">通用修补建议微软已发布相关安全更新，用户可跟进以下链接进行升级:CVE-2021-26855:https://msrc.microsoft.com/update-guide/vulnerability/CVE-2021-26855CVE-2021-26857:https://msrc.microsoft.com/update-guide/vulnerability/CVE-2021-26855CVE-2021-26858:https://msrc.microsoft.com/update-guide/vulnerability/CVE-2021-26855CVE-2021-27065:https://msrc.microsoft.com/update-guide/vulnerability/CVE-2021-26855临时修补建议CVE-2021-26855：可以通过以下Exchange HttpProxy日志进行检测：%PROGRAMFILES%\Microsoft\Exchange Server\V15\Logging\HttpProxy通过以下Powershell可直接进行日志检测，并检查是否受到攻击：Import-Csv -Path (Get-ChildItem -Recurse -Path “$env:PROGRAMFILES\Microsoft\Exchange Server\V15\Logging\HttpProxy” -Filter ‘*.log’).FullName | Where-Object {  $_.AuthenticatedUser -eq ” -and $_.AnchorMailbox -like ‘ServerInfo~*/*’ } | select DateTime, AnchorMailbox
+如果检测到了入侵，可以通过以下目录获取攻击者采取了哪些活动%PROGRAMFILES%\Microsoft\Exchange Server\V15\LoggingCVE-2021-26858：日志目录：C:\Program Files\Microsoft\Exchange Server\V15\Logging\OABGeneratorLog可通过以下命令进行快速浏览，并检查是否受到攻击：findstr /snip /c:”Download failed and temporary file” “%PROGRAMFILES%\Microsoft\Exchange Server\V15\Logging\OABGeneratorLog\*.log”
+CVE-2021-26857：该漏洞单独利用难度稍高，可利用以下命令检测日志条目，并检查是否受到攻击。Get-EventLog -LogName Application -Source “MSExchange Unified Messaging” -EntryType Error | Where-Object { $_.Message -like “*System.InvalidCastException*” }
+CVE-2021-27065:通过以下powershell命令进行日志检测，并检查是否遭到攻击:Select-String -Path “$env:PROGRAMFILES\Microsoft\Exchange Server\V15\Logging\ECP\Server\*.log” -Pattern ‘Set-.+VirtualDirectory’
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-02-26</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SaltStack 多个高危漏洞通告</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://cert.360.cn/warning/detail?id=3c9c30d8b1bcf14b7697a40d5f70489d</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2021年02月26日，360CERT监测发现SaltStack发布了2月份安全更新的风险通告 ，事件等级：高危，事件评分：8.1。SaltStack在本次更新中修复了 10 个漏洞，其中包含6个高危漏洞。对此，360CERT建议广大用户及时将SaltStack升级到最新版本。与此同时，请做好资产自查以及预防工作，以免遭受黑客攻击。</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CVE-2021-3197: 命令注入在安装并开启 SSH 模块的SaltStack服务器存在一处命令注入漏洞。攻击者可以通过Salt-API 的 SSH功能接口使用 SSH 命令的ProxyCommand参数进行命令注入。CVE-2021-25281: 代码执行SaltStack SaltAPI中存在一处代码执行漏洞。wheel_async模块未正确处理身份验证请求，导致攻击者利用该模块执行任意 python 代码。CVE-2021-25282: 目录穿越SaltStack SaltAPI中存在一处代码执行漏洞。该漏洞主要是salt.wheel.pillar_roots.write函数在写入操作时存在目录穿越，与CVE-2021-25281、CVE-2021-25283结合实现代码执行。CVE-2021-25283: 代码执行SaltStack jinja模板渲染中存在一处代码执行漏洞。该漏洞主要是salt.wheel.pillar_roots.write函数在写入操作时，将存在恶意代码的模板文件写入特定位置，在请求相关页面时触发 jinja 引擎渲染导致代码执行与CVE-2021-25282结合实现代码执行。CVE-2021-3148: 命令注入SaltAPIsalt.utils.thin.gen_thin()方法存在一处命令注入漏洞。攻击者可以利用插入单引号'实现命令注入，该漏洞与json.dumps不对处理输入内容中单引号也存在关联。</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>通用修补建议注意 SaltStack 未针对该此更新发布新的版本号，建议用户前往控制台自行更新，或者手动从官方仓库获取最新版本的 SaltStack。升级到- SaltStack：3002.5/3001.6/3000.8下载地址为：SaltStack Release。</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2021-02-24</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>VMware多个高危漏洞通告</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://cert.360.cn/warning/detail?id=ed5c81bdac7ed43ef70368590fdc8a2a</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2021年02月24日，360CERT监测发现VMware发布了Vcenter Server、ESXI的风险通告，事件等级：严重，事件评分：9.8。VMware更新了ESXI和vSphere Client(HTML5)中的两个高危漏洞，具有网络端口访问权限的恶意攻击者可以通过漏洞执行任意代码。对此，360CERT建议广大用户及时将Vcenter Server与ESXI产品升级到最新版本。与此同时，请做好资产自查以及预防工作，以免遭受黑客攻击。</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CVE-2021-21972: 代码执行漏洞具有443端口访问权限的恶意攻击者可以通过向vCenter Server发送精心构造的请求，最终造成远程任意代码执行。CVE-2021-21974: 堆溢出漏洞与ESXI处于同一网段且可以访问427端口的恶意攻击者可以构造恶意请求包触发OpenSLP服务中的堆溢出漏洞，最终造成远程代码执行。</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>通用修补建议CVE-2021-21972：- vCenter Server7.0版本升级到7.0.U1c- vCenter Server6.7版本升级到6.7.U3l- vCenter Server6.5版本升级到6.5 U3nCVE-2021-21974：- ESXi7.0版本升级到ESXi70U1c-17325551- ESXi6.7版本升级到ESXi670-202102401-SG- ESXi6.5版本升级到ESXi650-202102101-SG临时修补建议CVE-2021-219721. SSH远连到vCSA（或远程桌面连接到Windows VC）2. 备份以下文件：- Linux系文件路径为：/etc/vmware/vsphere-ui/compatibility-matrix.xml (vCSA)- Windows文件路径为：C:\ProgramData\VMware\vCenterServer\cfg\vsphere-ui (Windows VC)3. 使用文本编辑器将文件内容修改为：4. 使用vmon-cli -r vsphere-ui命令重启vsphere-ui服务
+5. 访问https://&lt;VC-IP-or-FQDN&gt;/ui/vropspluginui/rest/services/checkmobregister，显示404错误6. 在vSphere Client的Solutions-&gt;Client Plugins中VMWare vROPS插件显示为incompatibleCVE-2021-219741. 使用/etc/init.d/slpd stop命令在ESXI主机上停止SLP服务（仅当不使用SLP服务时，才可以停止该服务。可以使用esxcli system slp stats get命令查看服务守护程序运行状态）
+2. 使用esxcli network firewall ruleset set -r CIMSLP -e 0命令禁用SLP服务
+3. 使用chkconfig slpd off命令保证此更改在重启后持续存在
+4. 利用chkconfig --list | grep slpd命令检查是否在重启后更改成功，若回显为slpd off则证明成功</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-03-03 14:22:42</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Microsoft Exchange多个高危漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/207</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近日，奇安信CERT监测到微软修复了Microsoft Exchange多个高危漏洞。通过组合利用这些漏洞能够在未经身份验证的情况下远程获取目标服务器权限。其中包括：
+CVE-2021-26855: 服务端请求伪造（SSRF）漏洞，通过该漏洞，攻击者可以发送任意HTTP请求并通过Exchange Server进行身份验证，获取权限。
+CVE-2021-26857: 是统一消息服务中的不安全反序列化漏洞。通过该此漏洞，具有管理员权限的攻击者可以在Exchange服务器上以SYSTEM身份运行任意代码。
+CVE-2021-26858/CVE-2021-27065: 任意文件写入漏洞，在通过身份验证后攻击者可以利用该漏洞将文件写入服务器的任意路径。
+目前微软称已经监测到了利用该漏洞进行攻击的事件，经过奇安信安全专家确认，漏洞无需验证和交互即可触发远程代码执行，危害极大，建议客户尽快自查修复。
+</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">使用奇安信天擎的客户可以通过奇安信天擎控制台一键更新修补相关漏洞，也可以通过奇安信天擎客户端一键更新修补相关漏洞。
+也可以采用以下官方解决方案及缓解方案来防护此漏洞：
+Windows自动更新
+Windows系统默认启用 Microsoft Update，当检测到可用更新时，将会自动下载更新并在下一次启动时安装。还可通过以下步骤快速安装更新：
+1、点击“开始菜单”或按Windows快捷键，点击进入“设置”
+2、选择“更新和安全”，进入“Windows更新”（Windows 8、Windows 8.1、Windows Server 2012以及Windows Server 2012 R2可通过控制面板进入“Windows更新”，步骤为“控制面板”-&gt; “系统和安全”-&gt;“Windows更新”）
+3、选择“检查更新”，等待系统将自动检查并下载可用更新
+4、重启计算机，安装更新
+系统重新启动后，可通过进入“Windows更新”-&gt;“查看更新历史记录”查看是否成功安装了更新。对于没有成功安装的更新，可以点击该更新名称进入微软官方更新描述链接，点击最新的SSU名称并在新链接中点击“Microsoft 更新目录”，然后在新链接中选择适用于目标系统的补丁进行下载并安装。
+手动安装补丁
+另外，对于不能自动更新的系统版本（如Windows 7、Windows Server 2008、Windows Server 2008 R2），可参考以下链接下载适用于该系统的补丁并安装：
+https://msrc.microsoft.com/update-guide/
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021-03-02 16:24:34</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SaltStack多个高危漏洞安全风险通告第二次更新</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/206</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近日，奇安信CERT监测到SaltStack官方发布安全更新修复了三个高危漏洞，通过组合这三个漏洞可以达到远程代码执行效果。
+SaltStack的REST API接口run中存在未授权访问漏洞（CVE-2021-25281）：攻击者可以向该接口发送发起异步调用，在异步调用中未作鉴权，从而绕过权限鉴定，执行salt的任意python模块，奇安信CERT第一时间复现，截图如下。
+ ![3.21.png](https://lxs3.b.qianxin.com/Webportal-image/2312)
+SaltStack的pillar_roots.write模块中存在任意文件写漏洞（CVE-2021-25282）：在该模块中，代码直接拼接了pillar_roots和用户传入的path，通过传入../可以达到目录遍历，从而在目标目录写入恶意文件，奇安信CERT第一时间复现，截图如下。
+ ![3.22.png](https://lxs3.b.qianxin.com/Webportal-image/2313)
+ ![3.23.png](https://lxs3.b.qianxin.com/Webportal-image/2314)
+ ![3.24.png](https://lxs3.b.qianxin.com/Webportal-image/2315)
+SaltStack的默认模板渲染引擎存在服务端模板注入漏洞（CVE-2021-25283）：通过配置sdb模块配置文件可以向Jinja2传递恶意payload，当salt-master加载配置文件时即可触发SSTI里面的恶意代码。奇安信CERT第一时间复现，截图如下。
+ ![3.25.png](https://lxs3.b.qianxin.com/Webportal-image/2316)
+ ![3.26.png](https://lxs3.b.qianxin.com/Webportal-image/2317)
+ ![3.27.png](https://lxs3.b.qianxin.com/Webportal-image/2319)
+通过组合上述三个漏洞即可达到远程代码执行的效果，截图如下。
+ ![3.28.png](9)
+ ![3.29.png](https://lxs3.b.qianxin.com/Webportal-image/2321)
+</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.SaltStack升级到 3002.3 / 3001.6 / 3000.8 或以上版本
+2.缓解措施：如果没有用到wheel_async模块，可以在salt/salt/netapi/__init__.py中将其删除，可以临时缓解未授权访问漏洞（CVE-2021-25281）
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021-03-01 11:16:32</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SaltStack多个高危漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/204</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近日，奇安信CERT监测到SaltStack官方发布安全更新修复了三个高危漏洞，通过组合这三个漏洞可以达到远程代码执行效果。
+SaltStack的REST API接口run中存在未授权访问漏洞（CVE-2021-25281）：攻击者可以向该接口发送发起异步调用，在异步调用中未作鉴权，从而绕过权限鉴定，执行salt的任意python模块，奇安信CERT第一时间复现，截图如下。
+ ![1.png](https://lxs3.b.qianxin.com/Webportal-image/2292)
+SaltStack的pillar_roots.write模块中存在任意文件写漏洞（CVE-2021-25282）：在该模块中，代码直接拼接了pillar_roots和用户传入的path，通过传入../可以达到目录遍历，从而在目标目录写入恶意文件，奇安信CERT第一时间复现，截图如下。
+ ![2.png](https://lxs3.b.qianxin.com/Webportal-image/2293)
+ ![3.png](https://lxs3.b.qianxin.com/Webportal-image/2294)
+ ![4.png](https://lxs3.b.qianxin.com/Webportal-image/2295)
+SaltStack的默认模板渲染引擎存在服务端模板注入漏洞（CVE-2021-25283）：通过配置sdb模块配置文件可以向Jinja2传递恶意payload，当salt-master加载配置文件时即可触发SSTI里面的恶意代码。
+通过组合上述三个漏洞即可达到远程代码执行的效果。
+</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.SaltStack升级到 3002.3 / 3001.6 / 3000.8 或以上版本
+2.缓解措施：如果没有用到wheel_async模块，可以在salt/salt/netapi/__init__.py中将其删除，可以临时缓解未授权访问漏洞（CVE-2021-25281）
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2021-02-25 14:40:04</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VMware产品多个高危漏洞安全风险通告第二次更新</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/203</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VMware vCenter Server远程代码执行漏洞（CVE-2021-21972）：vSphere Client（HTML5）在vCenter Server插件中存在一个远程执行代码漏洞。未授权的攻击者可以通过开放 443 端口的服务器向 vCenter Server 发送精心构造的请求，从而在服务器上写入webshell，最终造成远程任意代码执行。
+VMware vCenter Server SSRF漏洞（CVE-2021-21973）：由于vCenter Server插件中URL的验证不正确，vSphere Client（HTML5）包含SSRF（服务器端请求伪造）漏洞。可通过端口443访问网络的恶意攻击者通过向vCenter Server插件发送POST请求来导致信息泄露。
+VMware ESXi堆溢出漏洞（CVE-2021-21974）：当在OpenSLP服务中处理数据包时，由于边界错误，本地网络上的远程非身份验证攻击者可以将伪造的数据包发送到端口427/tcp，触发基于堆的缓冲区溢出，并在目标系统上执行任意代码。
+奇安信CERT第一时间复现CVE-2021-21972漏洞，复现截图如下：
+ ![2.251.png](https://lxs3.b.qianxin.com/Webportal-image/2279)
+</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.VMware vCenter Server远程代码执行漏洞（CVE-2021-21972）和
+VMware vCenter Server SSRF漏洞（CVE-2021-21973）
+- 升级到安全版本：
+vCenter Server 7.0 版本升级到 7.0.U1c
+vCenter Server 6.7 版本升级到 6.7.U3l
+vCenter Server 6.5 版本升级到 6.5 U3n
+- 缓解措施：
+a)SSH连接到vCSA（或远程桌面连接到Windows VC）
+b)备份以下文件：
+- Linux系统文件路径：
+```/etc/vmware/vsphere-ui/compatibility-matrix.xml (vCSA)
+```
+- Windows系统文件路径：
+```
+C:\ProgramData\VMware\vCenterServer\cfg\vsphere-ui (Windows VC)
+```
+c)使用文本编辑器插入：
+```
+&lt;Matrix&gt;
+&lt;pluginsCompatibility&gt;
+  . . . . 
+  . . . . 
+&lt;PluginPackage id="com.vmware.vrops.install" status="incompatible"/&gt;
+&lt;/pluginsCompatibility&gt;
+&lt;/Matrix&gt;
+```
+将文件内容修改为下图所示：
+ ![2.241.png](https://lxs3.b.qianxin.com/Webportal-image/2280)
+d)使用vmon-cli -r vsphere-ui命令重启vsphere-ui服务
+e)访问https://&lt;VC-IP-or-FQDN&gt;/ui/vropspluginui/rest/services/checkmobregister，显示404错误
+ ![2.242.png](https://lxs3.b.qianxin.com/Webportal-image/2281)
+f)在vSphere Client的Solutions-&gt;Client Plugins中VMWare vROPS插件显示为incompatible
+ ![2.243.png](https://lxs3.b.qianxin.com/Webportal-image/2282)
+2.VMware ESXi堆溢出漏洞（CVE-2021-21974）
+- 升级到安全版本：
+ESXi 7.0 版本升级到 ESXi70U1c-17325551 
+ESXi 6.7 版本升级到 ESXi670-202102401-SG
+ESXi 6.5 版本升级到 ESXi650-202102101-SG
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-03-01 14:19:09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>VMware产品多个高危漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/202</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VMware vCenter Server远程代码执行漏洞（CVE-2021-21972）：vSphere Client（HTML5）在vCenter Server插件中存在一个远程执行代码漏洞。未授权的攻击者可以通过开放 443 端口的服务器向 vCenter Server 发送精心构造的请求，从而在服务器上写入webshell，最终造成远程任意代码执行。
+VMware ESXi堆溢出漏洞（CVE-2021-21974）：当在OpenSLP服务中处理数据包时，由于边界错误，本地网络上的远程非身份验证攻击者可以将伪造的数据包发送到端口427/tcp，触发基于堆的缓冲区溢出，并在目标系统上执行任意代码。
+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.VMware vCenter Server远程代码执行漏洞（CVE-2021-21972） 
+- 升级到安全版本：
+vCenter Server 7.0 版本升级到 7.0.U1c
+vCenter Server 6.7 版本升级到 6.7.U3l
+vCenter Server 6.5 版本升级到 6.5 U3n
+- 缓解措施：
+a)SSH连接到vCSA（或远程桌面连接到Windows VC）
+b)备份以下文件：
+- Linux系统文件路径：
+```
+/etc/vmware/vsphere-ui/compatibility-matrix.xml (vCSA)
+```
+- Windows系统文件路径：
+```
+C:\ProgramData\VMware\vCenterServer\cfg\vsphere-ui (Windows VC)
+```
+c)使用文本编辑器插入：
+```
+&lt;Matrix&gt;
+&lt;pluginsCompatibility&gt;
+  . . . . 
+  . . . . 
+&lt;PluginPackage id="com.vmware.vrops.install" status="incompatible"/&gt;
+&lt;/pluginsCompatibility&gt;
+&lt;/Matrix&gt;
+```
+将文件内容修改为下图所示：
+ ![2.241.png](https://lxs3.b.qianxin.com/Webportal-image/2272)
+d)使用vmon-cli -r vsphere-ui命令重启vsphere-ui服务
+e)访问https://&lt;VC-IP-or-FQDN&gt;/ui/vropspluginui/rest/services/checkmobregister，显示404错误
+ ![2.242.png](https://lxs3.b.qianxin.com/Webportal-image/2275)
+f)在vSphere Client的Solutions-&gt;Client Plugins中VMWare vROPS插件显示为incompatible
+ ![2.243.png](https://lxs3.b.qianxin.com/Webportal-image/2276)
+2.VMware ESXi堆溢出漏洞（CVE-2021-21974）
+- 升级到安全版本：
+ESXi 7.0 版本升级到 ESXi70U1c-17325551 
+ESXi 6.7 版本升级到 ESXi670-202102401-SG
+ESXi 6.5 版本升级到 ESXi650-202102101-SG
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-02-25 11:34:18</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Windows TCP/IP多个高危漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/201</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近日，微软发布2月份的漏洞补丁程序，其中包含3个Windows TCP/IP漏洞，这些漏洞无需交互及身份认证，可远程触发，成功利用这些漏洞可导致目标系统宕机或远程代码执行，具体如下表所示：
+|CVE编号|风险等级|漏洞名称|利用可能|
+| -- | -- | -- | -- |
+|CVE-2021-24074|紧急|Windows TCP/IP 远程代码执行漏洞|N/N/M|
+|CVE-2021-24094|紧急|Windows TCP/IP 远程代码执行漏洞|N/N/M|
+|CVE-2021-24086|重要|Windows TCP/IP拒绝服务漏洞|N/N/M|
+注：“利用可能”字段包含四个维度（是否公开[Y/N]/是否在野利用[Y/N]/可利用性评估[D/M/L/U/NA]）
+|简写|定义|翻译|
+| -- | -- | -- |
+|Y|Yes|是|
+|N|No|否|
+|D|0-Exploitation detected|0-检测到利用|
+|M|1-Exploitation more likely *	|1-被利用可能性极大|
+|L|2-Exploitation less likely **|2-被利用可能性一般|
+|U|3-Exploitation unlikely ***|3-被利用可能性很小|
+|NA|4-N/A|4-不适用|
+- CVE-2021-24074：
+Windows IPv4 协议栈存在一处远程代码执行漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功的利用可能允许攻击者在目标系统上执行任意代码。
+- CVE-2021-24094：
+Windows IPv6协议栈存在一处远程代码执行漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功利用此漏洞可导致目标系统拒绝服务（蓝屏）或潜在的任意代码执行。
+- CVE-2021-24086：
+Windows IPv6协议栈存在一处拒绝服务漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功利用此漏洞可导致目标系统拒绝服务（蓝屏）。
+</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**奇安信天擎终端安全管理系统解决方案**
+奇安信已第一时间提供热补丁工具，热补丁无需重启系统即可生效防护，下载地址：https://www.qianxin.com/other/win10-BadCon-CondrvVulFix
+ ![2.101.png](https://lxs3.b.qianxin.com/Webportal-image/2271)
+奇安信天擎终端安全管理系统并且有漏洞修复相关模块的用户，可以将补丁库版本更新到：2021.02.10.1及以上版本，对内网终端进行补丁更新。
+推荐采用自动化运维方案，如果控制中心可以连接互联网的用户场景，建议设置为自动从奇安信云端更新补丁库至2021.02.10.1版本。
+控制中心补丁库更新方式：每天04:00-06:00自动升级，升级源为从互联网升级。
+纯隔离网内控制中心不能访问互联网，不能下载补丁库和补丁文件，需使用离线升级工具定期导入补丁库和文件到控制中心。
+**奇安信天眼产品解决方案**
+微软2月份补丁日修复了一批Windows TCP/IP漏洞，奇安信天眼新一代威胁感知系统在第一时间加入了这些漏洞的检测规则，请将规则包升级到3.0.0210.12641及以上版本。规则名称：Windows TCP/IP 协议栈远程代码执行漏洞(CVE-2021-24074)，规则ID：0x5da1；规则名称：Windows TCP/IP 协议栈拒绝服务漏洞(CVE-2021-24086)，规则ID：0x5d9f ；规则名称：Windows TCP/IP 协议栈远程代码执行漏洞(CVE-2021-24094)，规则ID：0x5da0。奇安信天眼流量探针（传感器）升级方法：系统配置-&gt;设备升级-&gt;规则升级，选择“网络升级”或“本地升级”。
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-02-25 11:23:08</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>微软2月补丁日多产品高危漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/200</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">本月，微软共发布56个漏洞的补丁程序，其中，CVE-2021-24078漏洞由奇安信代码安全实验室发现并提交。另外，CVE-2021-1732 Windows Win32k权限提升漏洞已检测到在野攻击，以下8个漏洞被微软标记为 “Exploitation More Likely”，这代表这些漏洞更容易被利用：
+- CVE-2021-24074
+- CVE-2021-24078
+- CVE-2021-24094
+- CVE-2021-1727
+- CVE-2021-1698
+- CVE-2021-24066
+- CVE-2021-24072
+- CVE-2021-24086
+奇安信CERT对此进行研判，影响较大的8个漏洞（包括3个紧急漏洞和5个重要漏洞）的详细信息如下：
+1、CVE-2021-24074 Windows TCP/IP 远程代码执行漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows TCP/IP 远程代码执行漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;远程代码执行&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;紧急&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-24074&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows IPv4 协议栈存在一处远程代码执行漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功的利用可能允许攻击者在目标系统上执行任意代码。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-24074&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+2、CVE-2021-24078 Windows DNS Server 远程代码执行漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows DNS Server 远程代码执行漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;远程代码执行&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;紧急&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-24078&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;攻击者仅需向目标DNS服务器发送特制数据包，即可利用该漏洞在目标系统上以本地系统账户权限执行任意代码，且触发无需交互、无需身份认证且在 Windows DNS 默认配置下即可执行。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-24078&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+3、CVE-2021-24094 Windows TCP/IP 远程代码执行漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows TCP/IP 远程代码执行漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;远程代码执行&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;紧急&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-24094&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows IPv6协议栈存在一处远程代码执行漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功利用此漏洞可导致目标系统拒绝服务（蓝屏）或潜在的任意代码执行。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-24094&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+4、CVE-2021-1732 Windows Win32k权限提升漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows Win32k 权限提升漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;权限提升&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;重要&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-1732&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows内核模式驱动对内存对象处理不当导致的权限提升漏洞。攻击成功将提升攻击者的特权，可能允许他们创建新帐户、安装程序和查看、修改或删除数据。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-1732&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+5、CVE-2021-1727 Windows Installer权限提升漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows Installer权限提升漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;权限提升&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;重要&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-1727&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows Installer中存在一枚权限提升漏洞。攻击者需要一个低特权的用户帐户，攻击成功将提升攻击者的特权，可能允许他们创建新帐户、安装程序和查看、修改或删除数据。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-1727&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+6、CVE-2021-1698 Windows Win32k权限提升漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows Win32k权限提升漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;权限提升&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;重要&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-1698&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;在Microsoft Windows中存在特权提升漏洞。成功利用此漏洞可以让远程攻击者在受影响的系统上执行任意代码。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-1698&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+7、CVE-2021-24072 Microsoft SharePoint Server远程代码执行漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;	Microsoft SharePoint Server远程代码执行漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;远程代码执行&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;重要&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-24072&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Microsoft SharePoint存在远程代码执行漏洞。成功利用此漏洞可以让远程攻击者在受影响的系统上执行任意代码。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-24072&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+8、CVE-2021-24086 Windows TCP/IP拒绝服务漏洞
+&lt;table&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞名称&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows TCP/IP拒绝服务漏洞&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞类型&lt;/td&gt;
+      &lt;td&gt;拒绝服务&lt;/td&gt;
+      &lt;td&gt;风险等级&lt;/td&gt;
+      &lt;td&gt;重要&lt;/td&gt;
+      &lt;td&gt;漏洞ID&lt;/td&gt;
+      &lt;td&gt;CVE-2021-24086&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;公开状态&lt;/td&gt;
+      &lt;td&gt;未公开&lt;/td&gt;
+      &lt;td&gt;在野利用&lt;/td&gt;
+      &lt;td colspan="3"&gt;未发现&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td&gt;漏洞描述&lt;/td&gt;
+      &lt;td colspan="5"&gt;Windows IPv6协议栈存在一处拒绝服务漏洞，远程攻击者可通过向目标系统发送特制数据包来利用此漏洞，成功利用此漏洞可导致目标系统拒绝服务（蓝屏）。&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;参考链接&lt;/td&gt;
+   &lt;/tr&gt;
+   &lt;tr&gt;
+      &lt;td colspan="6"&gt;https://portal.msrc.microsoft.com/en-US/security-guidance/advisory/CVE-2021-24086&lt;/td&gt;
+   &lt;/tr&gt;
+&lt;/table&gt;
+&lt;br/&gt;
+</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**奇安信天擎终端安全管理系统解决方案**
+微软2月安全更新修补了多个已公开PoC的0day漏洞，需要用户尽快修补。其中包括：
+1、CVE-2021-24094/CVE-2021-24074/CVE-2021-24086，3个涉及Windows TCP/IP高危漏洞。
+2、CVE-2021-24098，ConDrv.sys拒绝服务（DoS）漏洞，该漏洞在Windows 10系统上会触发蓝屏（BSOD）。
+奇安信已第一时间提供热补丁工具，热补丁无需重启系统即可生效防护，下载地址：https://www.qianxin.com/other/win10-BadCon-CondrvVulFix
+ ![2.102.png](https://lxs3.b.qianxin.com/Webportal-image/2268)
+3、CVE-2021-1727，Windows Installer特权提升漏洞，详细信息请参考“奇安信CERT”公众号发布的公告。
+https://mp.weixin.qq.com/s/VFSCkCeuaHRlaxWV0-jbHA
+奇安信天擎终端安全管理系统并且有漏洞修复相关模块的用户，可以将补丁库版本更新到：2021.02.10.1及以上版本，对内网终端进行补丁更新。
+推荐采用自动化运维方案，如果控制中心可以连接互联网的用户场景，建议设置为自动从奇安信云端更新补丁库至2021.02.10.1版本。
+控制中心补丁库更新方式：每天04:00-06:00自动升级，升级源为从互联网升级。
+纯隔离网内控制中心不能访问互联网，不能下载补丁库和补丁文件，需使用离线升级工具定期导入补丁库和文件到控制中心。
+**奇安信天眼产品解决方案**
+微软2月份补丁日修复了一批漏洞，奇安信天眼新一代威胁感知系统在第一时间加入了这些漏洞的检测规则，请将规则包升级到3.0.0210.12641及以上版本。
+规则名称：Microsoft SharePoint远程代码执行漏洞(CVE-2021-24072)，规则ID：0x10020BCF；规则名称：Microsoft DNS服务器代码执行漏洞(CVE-2021-24078)，规则ID：0x5d9e；规则名称：Windows TCP/IP 协议栈远程代码执行漏洞(CVE-2021-24074)，规则ID：0x5da1；规则名称：Windows TCP/IP 协议栈拒绝服务漏洞(CVE-2021-24086)，规则ID：0x5d9f ；规则名称：Windows TCP/IP 协议栈远程代码执行漏洞(CVE-2021-24094)，规则ID：0x5da0。
+奇安信天眼流量探针（传感器）升级方法：系统配置-&gt;设备升级-&gt;规则升级，选择“网络升级”或“本地升级”。
+**奇安信网神网络数据传感器系统产品检测方案**
+奇安信网神网络数据传感器（NDS3000/5000/9000系列）产品，已具备该该补丁日多个高危漏洞（含：CVE-2021-24072、CVE-2021-24078）的检测能力。对应的规则ID为：6214、60242 ，建议用户尽快升级检测规则库至2102100900以后版本并启用该多个检测规则。
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-02-07 14:30:45</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>谷歌 V8 JavaScript引擎堆溢出漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/196</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">近日，谷歌官方发布最新的 Chrome 正式版本（88.0.4324.150），修复了关于谷歌 V8 JavaScript 引擎的堆溢出漏洞（CVE-2021-21148），该漏洞影响 Chrome 浏览器以及基于 Chromium 开发的版本低于 88.0.705.63 的 Microsoft Edge 浏览器。如若成功利用此漏洞，可能造成远程代码执行。据传该漏洞正在被广泛利用，目前暂未有更多细节披露，建议用户及时安装更新补丁。
+</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1、升级Chrome 浏览器至 88.0.4324.150 版本：
+Chrome 浏览器中打开 chrome://settings/help ，检查更新，升级，重新启动浏览器即可。
+2、更新 Microsoft Edge 浏览器至88.0.705.63版本：
+ Microsoft Edge 浏览器中打开edge://settings/help ，检查更新，升级，重新启动浏览器即可。
+或直接下载最新版本：https://www.microsoftedgeinsider.com/en-gb/download
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-02-02 19:57:01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Apache Shiro 身份认证绕过漏洞 安全风险通告</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/195</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Apache Shiro 是一个开源安全框架，拥有身份验证、授权、加密和会话管理的功能。当它和 Spring 结合使用时，在一定权限匹配规则下，攻击者可通过构造特殊的 HTTP 请求包完成身份认证绕过。
+奇安信 CERT 第一时间复现了 CVE-2020-17523 漏洞，复现截图如下：
+ ![复现截图1.png](https://lxs3.b.qianxin.com/Webportal-image/2203)
+ ![复现截图2.png](https://lxs3.b.qianxin.com/Webportal-image/2204)
+</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">升级到 Apache Shiro 1.7.1 。更新链接：https://github.com/apache/shiro/releases/tag/shiro-root-1.7.1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021-02-02 18:20:38</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Apache Druid远程代码执行漏洞安全风险通告</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://nox.qianxin.com/article/194</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">奇安信 CERT风险评级为：高危
+风险等级：蓝色（一般事件）
+&lt;br/&gt;
+</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**奇安信天眼产品解决方案**
+奇安信天眼新一代威胁感知系统在第一时间加入了该漏洞的检测规则，请将规则包升级到3.0.0202.12625上版本。规则名称：Apache Druid 远程代码执行漏洞，规则ID：0x10020BC5。奇安信天眼流量探针（传感器）升级方法：系统配置-&gt;设备升级-&gt;规则升级，选择“网络升级”或“本地升级”。
+**奇安信网神统一服务器安全管理平台更新入侵防御规则库**
+奇安信网神统一服务器安全管理平台轻代理版本可通过更新入侵防御规则库2021.02.05版本，支持对Apache Druid 0.20.0远程代码执行漏洞的防护，当前规则正在测试中，将于2月5日发布，届时请用户联系技术支持人员获取规则升级包对轻代理版本进行升级。
+奇安信网神统一服务器安全管理平台融合版本可通过更新入侵防御规则库10330版本，支持对Apache Druid 0.20.0远程代码执行漏洞的防护，当前规则正在测试中，将于2月5日发布，届时请用户联系技术支持人员获取规则升级包对融合版本进行升级。
+**奇安信网站应用安全云防护系统已更新防护特征库**
+奇安信网神网站应用安全云防护系统已全局更新所有云端防护节点的防护规则，支持对Apache Druid 0.20.0远程代码执行漏洞的防护。
+**奇安信网神智慧防火墙产品防护方案**
+奇安信新一代智慧防火墙（NSG3000/5000/7000/9000系列）和下一代极速防火墙（NSG3500/5500/7500/9500系列）产品系列，已通过更新IPS特征库完成了对该漏洞的防护。建议用户尽快将IPS特征库升级至” 2102021400” 及以上版本并启用规则ID: 1233001进行检测。
+**奇安信网神网络数据传感器系统产品检测方案**
+奇安信网神网络数据传感器（NDS3000/5000/9000系列）产品，已具备该漏洞的检测能力。规则ID为：6211，建议用户尽快升级检测规则库至2102021440以后版本并启用该检测规则。
+**奇安信开源卫士已更新**
+奇安信开源卫士20210202. 580版本已支持对Apache Druid 远程代码执行漏洞（CVE-2021-25646）的检测。
+&lt;br/&gt;
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>VMware View Planner 远程代码执行漏洞(CVE-2021-21978)风险通告</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1263.html</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2021年03月02日，VMware官方发布安全公告，通报了View Planner存在的一个安全高危漏洞风险，View Planner 在处理上传文件时存在一处漏洞。该漏洞允许攻击者上传文件至任意目录，并在特定情况下导致远程代码执行，该漏洞POC（概念验证代码）已在互联网上公开。</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+VMware
+View Planner 的 web 上传接口中itrLogPath参数未进行严格的校验，允许攻击者实施目录穿越，将文件上传至任意目录。在攻击者上传恶意脚本文件覆盖特定的 web 程序执行脚本时，可造成远程代码执行。
+</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>微软Exchange多个高危漏洞通告，腾讯安全建议用户尽快修复</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1261.html</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>微软紧急发布了Exchange 多个高危漏洞的风险通告，按常规进度，该漏洞会在3月份的例行安全公告中发布，因漏洞影响严重，已有在野攻击利用，微软已提前发布漏洞补丁，微软提前发布安全补丁的事件十分少见，表明该漏洞的危险等级十分严重。腾讯安全专家建议受影响的政企用户尽快升级修复。</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+CVE-2021-26855: 服务端请求伪造漏洞
+</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Apache Tomcat HTTP/2 cleartext (H2C) 请求混合漏洞（CVE-2021-25122）风险通告</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1260.html</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Apache Tomcat 官方于3月1日发布一个安全漏洞公告（CVE-2021-25122），漏洞风险等级为“重要”。Apache Tomcat 在响应新的h2c连接请求时，可以将请求标头和数量有限的请求主体从一个请求复制到另一个请求，这意味着用户A和用户B都可以看到用户A的请求结果。</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saltstack高危漏洞（CVE-2021-25281等）风险通告，腾讯安全全面检测 </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1258.html</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2021年2月25日，SaltStack发布安全更新，修复了由腾讯安全云鼎实验室提交的三个安全漏洞。利用这些漏洞，最严重情形可导致未授权远程代码执行。SaltStack套件已是政企机构 IT运维管理人员常用的管理工具，该组件的高危漏洞风险极大，值得高度关注。腾讯安全专家建议Saltstack用户尽快修复漏洞，避免黑客入侵后造成严重损失。</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+本次披露的高危漏洞包括以下几个：
+</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>VMware 多个高危漏洞（CVE-2021-21972，CVE-2021-21973，CVE-2021-21974）风险通告，腾讯御界支持检测</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1255.html</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>VMware 官方发布公告，修复了ESXi和vSphere Client（HTML5）中的多个高危漏洞，攻击者利用漏洞可能导致远程代码执行或信息泄露，腾讯高级威胁检测系统（御界）已支持检测利用VM相关漏洞的攻击活动。</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+1.vSphere Client中的远程执行代码漏洞（CVE-2021-21972）
+</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TCP/IP远程代码执行漏洞影响全系列Windows系统，腾讯安全提供全面解决方案</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1252.html</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2021年2月10日，Microsoft在2月例行补丁日发布了2个TCP/IP高危漏洞（CVE-2021-24074/CVE-2021- 24086）的补丁。腾讯安全团队已第一时间对本次修复的漏洞进行分析，腾讯主机安全（云镜）、零信任无边界访问控制系统（iOA）已支持检测该漏洞，腾讯云防火墙、高级威胁检测系统（御界）已支持对检测该漏洞的利用攻击。</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>微软发布2021年2月安全更新</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1251.html</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2021年2月10日，微软发布了2021年2月例行安全更新，本次发布包括.net、Office、Edga浏览器、Windows等多个常用软件的安全更新。</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2021-03-05 09:15:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Apache Ambari任意文件下载漏洞（CVE-2020-13924）风险通告</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://s.tencent.com//research/bsafe/1250.html</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2021年2月7日，Apache官方公告了一个 Apache Ambari任意文件下载漏洞。Ambari 的鉴权模块存在设计缺陷，恶意用户可以绕过身份验证，进行目录遍历和下载任意文件。</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>